<commit_message>
update analysis with GW4 data
</commit_message>
<xml_diff>
--- a/results/Forwards_analysis.xlsx
+++ b/results/Forwards_analysis.xlsx
@@ -38,7 +38,7 @@
       <color rgb="00F1F1F1"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="13">
     <fill>
       <patternFill/>
     </fill>
@@ -52,17 +52,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00DC143C"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="00228B22"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00CCECE6"/>
+        <fgColor rgb="00DC143C"/>
       </patternFill>
     </fill>
     <fill>
@@ -82,7 +77,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0040AD75"/>
+        <fgColor rgb="00CCECE6"/>
       </patternFill>
     </fill>
     <fill>
@@ -92,17 +87,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0094BCA7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="00F2F1F1"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00E6979D"/>
+        <fgColor rgb="00E6959B"/>
       </patternFill>
     </fill>
     <fill>
@@ -129,24 +119,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -608,36 +596,36 @@
         <v>4.554709316290477</v>
       </c>
       <c r="E2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F2" s="3" t="n">
-        <v>5.333333333333333</v>
+        <v>8.25</v>
       </c>
       <c r="G2" t="n">
-        <v>-0.1694794927528091</v>
+        <v>0.4708833633870658</v>
       </c>
       <c r="H2" t="n">
-        <v>2.629662649840804</v>
+        <v>2.277354658145239</v>
       </c>
       <c r="I2" t="n">
-        <v>-0.2935470922888667</v>
+        <v>0.9417667267741316</v>
       </c>
       <c r="J2" t="n">
-        <v>0.398381460167222</v>
-      </c>
-      <c r="K2" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L2" s="4" t="inlineStr">
-        <is>
-          <t>Very small</t>
+        <v>0.2078945421187053</v>
+      </c>
+      <c r="K2" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="L2" s="5" t="inlineStr">
+        <is>
+          <t>Small</t>
         </is>
       </c>
       <c r="M2" s="2" t="n">
         <v>14</v>
       </c>
-      <c r="N2" s="5" t="n">
-        <v>2.666666666666667</v>
+      <c r="N2" s="6" t="n">
+        <v>2.75</v>
       </c>
     </row>
     <row r="3">
@@ -656,27 +644,27 @@
         <v>2.851061463238469</v>
       </c>
       <c r="E3" t="n">
-        <v>3</v>
-      </c>
-      <c r="F3" s="6" t="n">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="F3" s="3" t="n">
+        <v>4.25</v>
       </c>
       <c r="G3" t="n">
-        <v>0.4799689765639826</v>
+        <v>0.2169090567164152</v>
       </c>
       <c r="H3" t="n">
-        <v>1.646061103276899</v>
+        <v>1.425530731619235</v>
       </c>
       <c r="I3" t="n">
-        <v>0.8313306534656535</v>
+        <v>0.4338181134328303</v>
       </c>
       <c r="J3" t="n">
-        <v>0.2466166808188637</v>
-      </c>
-      <c r="K3" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L3" s="7" t="inlineStr">
+        <v>0.3468622549761498</v>
+      </c>
+      <c r="K3" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="L3" s="5" t="inlineStr">
         <is>
           <t>Small</t>
         </is>
@@ -684,8 +672,8 @@
       <c r="M3" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="N3" s="8" t="n">
-        <v>3</v>
+      <c r="N3" s="7" t="n">
+        <v>3.25</v>
       </c>
     </row>
     <row r="4">
@@ -704,27 +692,27 @@
         <v>2.83492443229031</v>
       </c>
       <c r="E4" t="n">
-        <v>3</v>
-      </c>
-      <c r="F4" s="3" t="n">
-        <v>1.666666666666667</v>
+        <v>4</v>
+      </c>
+      <c r="F4" s="4" t="n">
+        <v>1.5</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.582560555302318</v>
+        <v>-0.6413510700575977</v>
       </c>
       <c r="H4" t="n">
-        <v>1.636744384115058</v>
+        <v>1.417462216145155</v>
       </c>
       <c r="I4" t="n">
-        <v>-1.009024480269153</v>
+        <v>-1.282702140115195</v>
       </c>
       <c r="J4" t="n">
-        <v>0.2095959242805289</v>
-      </c>
-      <c r="K4" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L4" s="9" t="inlineStr">
+        <v>0.144860238210188</v>
+      </c>
+      <c r="K4" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="L4" s="8" t="inlineStr">
         <is>
           <t>Medium</t>
         </is>
@@ -732,8 +720,8 @@
       <c r="M4" s="2" t="n">
         <v>7.4</v>
       </c>
-      <c r="N4" s="10" t="n">
-        <v>3.333333333333333</v>
+      <c r="N4" s="7" t="n">
+        <v>3.25</v>
       </c>
     </row>
     <row r="5">
@@ -752,36 +740,36 @@
         <v>2.846974386589162</v>
       </c>
       <c r="E5" t="n">
-        <v>3</v>
-      </c>
-      <c r="F5" s="6" t="n">
-        <v>4.333333333333333</v>
+        <v>4</v>
+      </c>
+      <c r="F5" s="3" t="n">
+        <v>4.75</v>
       </c>
       <c r="G5" t="n">
-        <v>0.4498466022099757</v>
+        <v>0.5962008049837693</v>
       </c>
       <c r="H5" t="n">
-        <v>1.643701428473223</v>
+        <v>1.423487193294581</v>
       </c>
       <c r="I5" t="n">
-        <v>0.7791571706399038</v>
+        <v>1.192401609967539</v>
       </c>
       <c r="J5" t="n">
-        <v>0.2587221767683669</v>
-      </c>
-      <c r="K5" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L5" s="7" t="inlineStr">
-        <is>
-          <t>Small</t>
+        <v>0.159411326517823</v>
+      </c>
+      <c r="K5" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="L5" s="8" t="inlineStr">
+        <is>
+          <t>Medium</t>
         </is>
       </c>
       <c r="M5" s="2" t="n">
         <v>6.5</v>
       </c>
-      <c r="N5" s="10" t="n">
-        <v>3.333333333333333</v>
+      <c r="N5" s="7" t="n">
+        <v>3.25</v>
       </c>
     </row>
     <row r="6">
@@ -800,27 +788,27 @@
         <v>2.217355782608345</v>
       </c>
       <c r="E6" t="n">
-        <v>3</v>
-      </c>
-      <c r="F6" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="F6" s="4" t="n">
         <v>0</v>
       </c>
       <c r="G6" t="n">
         <v>-1.240215946204668</v>
       </c>
       <c r="H6" t="n">
-        <v>1.280190957978101</v>
+        <v>1.108677891304173</v>
       </c>
       <c r="I6" t="n">
-        <v>-2.148117031183594</v>
+        <v>-2.480431892409335</v>
       </c>
       <c r="J6" t="n">
-        <v>0.08237884256914314</v>
-      </c>
-      <c r="K6" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L6" s="11" t="inlineStr">
+        <v>0.04461792188866465</v>
+      </c>
+      <c r="K6" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="L6" s="9" t="inlineStr">
         <is>
           <t>Very large</t>
         </is>
@@ -828,8 +816,8 @@
       <c r="M6" s="2" t="n">
         <v>4.9</v>
       </c>
-      <c r="N6" s="12" t="n">
-        <v>3.666666666666667</v>
+      <c r="N6" s="10" t="n">
+        <v>3.5</v>
       </c>
     </row>
     <row r="7">
@@ -848,36 +836,36 @@
         <v>3.316051302802693</v>
       </c>
       <c r="E7" t="n">
-        <v>3</v>
-      </c>
-      <c r="F7" s="3" t="n">
-        <v>0.3333333333333333</v>
+        <v>4</v>
+      </c>
+      <c r="F7" s="4" t="n">
+        <v>1.25</v>
       </c>
       <c r="G7" t="n">
-        <v>-0.7221651969260112</v>
+        <v>-0.4457319988352853</v>
       </c>
       <c r="H7" t="n">
-        <v>1.914523112319744</v>
+        <v>1.658025651401347</v>
       </c>
       <c r="I7" t="n">
-        <v>-1.250826812533835</v>
+        <v>-0.8914639976705706</v>
       </c>
       <c r="J7" t="n">
-        <v>0.168744001146245</v>
-      </c>
-      <c r="K7" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L7" s="9" t="inlineStr">
-        <is>
-          <t>Medium</t>
+        <v>0.219178577887749</v>
+      </c>
+      <c r="K7" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="L7" s="5" t="inlineStr">
+        <is>
+          <t>Small</t>
         </is>
       </c>
       <c r="M7" s="2" t="n">
         <v>7.9</v>
       </c>
-      <c r="N7" s="8" t="n">
-        <v>3</v>
+      <c r="N7" s="7" t="n">
+        <v>3.25</v>
       </c>
     </row>
     <row r="8">
@@ -896,27 +884,27 @@
         <v>3.374838631159804</v>
       </c>
       <c r="E8" t="n">
+        <v>4</v>
+      </c>
+      <c r="F8" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="F8" s="3" t="n">
-        <v>2.333333333333333</v>
-      </c>
       <c r="G8" t="n">
-        <v>-0.1143654421628035</v>
+        <v>0.08317486702749352</v>
       </c>
       <c r="H8" t="n">
-        <v>1.948463992171661</v>
+        <v>1.687419315579902</v>
       </c>
       <c r="I8" t="n">
-        <v>-0.1980867564560556</v>
+        <v>0.166349734054987</v>
       </c>
       <c r="J8" t="n">
-        <v>0.4306428164957077</v>
-      </c>
-      <c r="K8" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L8" s="4" t="inlineStr">
+        <v>0.4392306165197497</v>
+      </c>
+      <c r="K8" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="L8" s="11" t="inlineStr">
         <is>
           <t>Very small</t>
         </is>
@@ -924,8 +912,8 @@
       <c r="M8" s="2" t="n">
         <v>7.9</v>
       </c>
-      <c r="N8" s="13" t="n">
-        <v>4</v>
+      <c r="N8" s="12" t="n">
+        <v>3.75</v>
       </c>
     </row>
     <row r="9">
@@ -944,36 +932,36 @@
         <v>2.564204284225516</v>
       </c>
       <c r="E9" t="n">
-        <v>3</v>
-      </c>
-      <c r="F9" s="6" t="n">
-        <v>4.333333333333333</v>
+        <v>4</v>
+      </c>
+      <c r="F9" s="3" t="n">
+        <v>3.75</v>
       </c>
       <c r="G9" t="n">
-        <v>0.6465532980508416</v>
+        <v>0.4190623228107307</v>
       </c>
       <c r="H9" t="n">
-        <v>1.480444033754793</v>
+        <v>1.282102142112758</v>
       </c>
       <c r="I9" t="n">
-        <v>1.119863162025281</v>
+        <v>0.8381246456214615</v>
       </c>
       <c r="J9" t="n">
-        <v>0.1896012602796353</v>
-      </c>
-      <c r="K9" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L9" s="9" t="inlineStr">
-        <is>
-          <t>Medium</t>
+        <v>0.2317403732356839</v>
+      </c>
+      <c r="K9" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="L9" s="5" t="inlineStr">
+        <is>
+          <t>Small</t>
         </is>
       </c>
       <c r="M9" s="2" t="n">
-        <v>6</v>
-      </c>
-      <c r="N9" s="8" t="n">
-        <v>3</v>
+        <v>6.1</v>
+      </c>
+      <c r="N9" s="6" t="n">
+        <v>2.75</v>
       </c>
     </row>
     <row r="10">
@@ -992,27 +980,27 @@
         <v>2.72065363800293</v>
       </c>
       <c r="E10" t="n">
-        <v>3</v>
-      </c>
-      <c r="F10" s="3" t="n">
-        <v>0.6666666666666666</v>
+        <v>4</v>
+      </c>
+      <c r="F10" s="4" t="n">
+        <v>0.75</v>
       </c>
       <c r="G10" t="n">
-        <v>-0.6835302725899632</v>
+        <v>-0.6529003782993752</v>
       </c>
       <c r="H10" t="n">
-        <v>1.570770110272726</v>
+        <v>1.360326819001465</v>
       </c>
       <c r="I10" t="n">
-        <v>-1.183909160637221</v>
+        <v>-1.30580075659875</v>
       </c>
       <c r="J10" t="n">
-        <v>0.1790449946717173</v>
-      </c>
-      <c r="K10" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L10" s="9" t="inlineStr">
+        <v>0.1413641843755108</v>
+      </c>
+      <c r="K10" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="L10" s="8" t="inlineStr">
         <is>
           <t>Medium</t>
         </is>
@@ -1020,8 +1008,8 @@
       <c r="M10" s="2" t="n">
         <v>5.9</v>
       </c>
-      <c r="N10" s="8" t="n">
-        <v>3</v>
+      <c r="N10" s="6" t="n">
+        <v>2.75</v>
       </c>
     </row>
     <row r="11">
@@ -1040,36 +1028,36 @@
         <v>2.834455750679565</v>
       </c>
       <c r="E11" t="n">
-        <v>3</v>
-      </c>
-      <c r="F11" s="6" t="n">
-        <v>3.333333333333333</v>
+        <v>4</v>
+      </c>
+      <c r="F11" s="3" t="n">
+        <v>4.5</v>
       </c>
       <c r="G11" t="n">
-        <v>0.3218539225866078</v>
+        <v>0.7334555735867889</v>
       </c>
       <c r="H11" t="n">
-        <v>1.63647379066093</v>
+        <v>1.417227875339782</v>
       </c>
       <c r="I11" t="n">
-        <v>0.557467346535345</v>
+        <v>1.466911147173578</v>
       </c>
       <c r="J11" t="n">
-        <v>0.3166372588899239</v>
-      </c>
-      <c r="K11" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L11" s="7" t="inlineStr">
-        <is>
-          <t>Small</t>
+        <v>0.1193391218209156</v>
+      </c>
+      <c r="K11" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="L11" s="8" t="inlineStr">
+        <is>
+          <t>Medium</t>
         </is>
       </c>
       <c r="M11" s="2" t="n">
         <v>7.3</v>
       </c>
-      <c r="N11" s="10" t="n">
-        <v>3.333333333333333</v>
+      <c r="N11" s="7" t="n">
+        <v>3.25</v>
       </c>
     </row>
     <row r="12">
@@ -1088,36 +1076,36 @@
         <v>2.796456341019272</v>
       </c>
       <c r="E12" t="n">
-        <v>3</v>
-      </c>
-      <c r="F12" s="6" t="n">
-        <v>4.666666666666667</v>
+        <v>4</v>
+      </c>
+      <c r="F12" s="3" t="n">
+        <v>4</v>
       </c>
       <c r="G12" t="n">
-        <v>0.8309836594704446</v>
+        <v>0.5925867079830219</v>
       </c>
       <c r="H12" t="n">
-        <v>1.614534821264513</v>
+        <v>1.398228170509636</v>
       </c>
       <c r="I12" t="n">
-        <v>1.439305918462324</v>
+        <v>1.185173415966044</v>
       </c>
       <c r="J12" t="n">
-        <v>0.143351434724561</v>
-      </c>
-      <c r="K12" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L12" s="14" t="inlineStr">
-        <is>
-          <t>Large</t>
+        <v>0.1606389983057708</v>
+      </c>
+      <c r="K12" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="L12" s="8" t="inlineStr">
+        <is>
+          <t>Medium</t>
         </is>
       </c>
       <c r="M12" s="2" t="n">
         <v>7.7</v>
       </c>
-      <c r="N12" s="13" t="n">
-        <v>4</v>
+      <c r="N12" s="12" t="n">
+        <v>3.75</v>
       </c>
     </row>
     <row r="13">
@@ -1136,36 +1124,36 @@
         <v>2.887777746459122</v>
       </c>
       <c r="E13" t="n">
-        <v>3</v>
-      </c>
-      <c r="F13" s="6" t="n">
-        <v>4</v>
+        <v>4</v>
+      </c>
+      <c r="F13" s="3" t="n">
+        <v>6</v>
       </c>
       <c r="G13" t="n">
-        <v>0.5741074564602312</v>
+        <v>1.266681530920193</v>
       </c>
       <c r="H13" t="n">
-        <v>1.667259259277985</v>
+        <v>1.443888873229561</v>
       </c>
       <c r="I13" t="n">
-        <v>0.9943832835932576</v>
+        <v>2.533363061840385</v>
       </c>
       <c r="J13" t="n">
-        <v>0.2124088424216217</v>
-      </c>
-      <c r="K13" s="3" t="b">
+        <v>0.04258640682909735</v>
+      </c>
+      <c r="K13" s="4" t="b">
         <v>0</v>
       </c>
       <c r="L13" s="9" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Very large</t>
         </is>
       </c>
       <c r="M13" s="2" t="n">
         <v>6.6</v>
       </c>
-      <c r="N13" s="5" t="n">
-        <v>2.666666666666667</v>
+      <c r="N13" s="6" t="n">
+        <v>2.75</v>
       </c>
     </row>
     <row r="14">
@@ -1184,27 +1172,27 @@
         <v>2.360506647838899</v>
       </c>
       <c r="E14" t="n">
-        <v>3</v>
-      </c>
-      <c r="F14" s="6" t="n">
-        <v>2.333333333333333</v>
+        <v>4</v>
+      </c>
+      <c r="F14" s="4" t="n">
+        <v>2</v>
       </c>
       <c r="G14" t="n">
-        <v>0.03908563648671487</v>
+        <v>-0.1021269856588352</v>
       </c>
       <c r="H14" t="n">
-        <v>1.36283914855369</v>
+        <v>1.18025332391945</v>
       </c>
       <c r="I14" t="n">
-        <v>0.06769830824115806</v>
+        <v>-0.2042539713176704</v>
       </c>
       <c r="J14" t="n">
-        <v>0.4760924103942012</v>
-      </c>
-      <c r="K14" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L14" s="4" t="inlineStr">
+        <v>0.4256133398415425</v>
+      </c>
+      <c r="K14" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="L14" s="11" t="inlineStr">
         <is>
           <t>Very small</t>
         </is>
@@ -1212,8 +1200,8 @@
       <c r="M14" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="N14" s="10" t="n">
-        <v>3.333333333333333</v>
+      <c r="N14" s="7" t="n">
+        <v>3.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update with GW5 data
</commit_message>
<xml_diff>
--- a/results/Forwards_analysis.xlsx
+++ b/results/Forwards_analysis.xlsx
@@ -38,7 +38,7 @@
       <color rgb="00F1F1F1"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill/>
     </fill>
@@ -67,12 +67,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="00228A44"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="0065C2A3"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00228A44"/>
       </patternFill>
     </fill>
     <fill>
@@ -92,12 +92,17 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00E6959B"/>
+        <fgColor rgb="00E6979D"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="00DA3B46"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0094BCA7"/>
       </patternFill>
     </fill>
   </fills>
@@ -119,7 +124,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -131,10 +136,11 @@
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -596,22 +602,22 @@
         <v>4.554709316290477</v>
       </c>
       <c r="E2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F2" s="3" t="n">
-        <v>8.25</v>
+        <v>7.8</v>
       </c>
       <c r="G2" t="n">
-        <v>0.4708833633870658</v>
+        <v>0.3720845227254851</v>
       </c>
       <c r="H2" t="n">
-        <v>2.277354658145239</v>
+        <v>2.036927929795419</v>
       </c>
       <c r="I2" t="n">
-        <v>0.9417667267741316</v>
+        <v>0.83200628618975</v>
       </c>
       <c r="J2" t="n">
-        <v>0.2078945421187053</v>
+        <v>0.2260961083317141</v>
       </c>
       <c r="K2" s="4" t="b">
         <v>0</v>
@@ -622,10 +628,10 @@
         </is>
       </c>
       <c r="M2" s="2" t="n">
-        <v>14</v>
+        <v>14.1</v>
       </c>
       <c r="N2" s="6" t="n">
-        <v>2.75</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="3">
@@ -644,22 +650,22 @@
         <v>2.851061463238469</v>
       </c>
       <c r="E3" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F3" s="3" t="n">
-        <v>4.25</v>
+        <v>4.4</v>
       </c>
       <c r="G3" t="n">
-        <v>0.2169090567164152</v>
+        <v>0.2695210406859287</v>
       </c>
       <c r="H3" t="n">
-        <v>1.425530731619235</v>
+        <v>1.275033447966247</v>
       </c>
       <c r="I3" t="n">
-        <v>0.4338181134328303</v>
+        <v>0.6026673683402233</v>
       </c>
       <c r="J3" t="n">
-        <v>0.3468622549761498</v>
+        <v>0.2896149239936908</v>
       </c>
       <c r="K3" s="4" t="b">
         <v>0</v>
@@ -673,7 +679,7 @@
         <v>8</v>
       </c>
       <c r="N3" s="7" t="n">
-        <v>3.25</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="4">
@@ -692,36 +698,36 @@
         <v>2.83492443229031</v>
       </c>
       <c r="E4" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F4" s="4" t="n">
-        <v>1.5</v>
+        <v>2.2</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.6413510700575977</v>
+        <v>-0.3944309080854226</v>
       </c>
       <c r="H4" t="n">
-        <v>1.417462216145155</v>
+        <v>1.267816748335227</v>
       </c>
       <c r="I4" t="n">
-        <v>-1.282702140115195</v>
+        <v>-0.8819743229059763</v>
       </c>
       <c r="J4" t="n">
-        <v>0.144860238210188</v>
+        <v>0.2138016944959831</v>
       </c>
       <c r="K4" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="L4" s="8" t="inlineStr">
-        <is>
-          <t>Medium</t>
+      <c r="L4" s="5" t="inlineStr">
+        <is>
+          <t>Small</t>
         </is>
       </c>
       <c r="M4" s="2" t="n">
-        <v>7.4</v>
+        <v>7.3</v>
       </c>
       <c r="N4" s="7" t="n">
-        <v>3.25</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="5">
@@ -740,36 +746,36 @@
         <v>2.846974386589162</v>
       </c>
       <c r="E5" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F5" s="3" t="n">
-        <v>4.75</v>
+        <v>4.2</v>
       </c>
       <c r="G5" t="n">
-        <v>0.5962008049837693</v>
+        <v>0.4030132573223619</v>
       </c>
       <c r="H5" t="n">
-        <v>1.423487193294581</v>
+        <v>1.273205651722827</v>
       </c>
       <c r="I5" t="n">
-        <v>1.192401609967539</v>
+        <v>0.9011650392064161</v>
       </c>
       <c r="J5" t="n">
-        <v>0.159411326517823</v>
+        <v>0.2092273859615639</v>
       </c>
       <c r="K5" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="L5" s="8" t="inlineStr">
-        <is>
-          <t>Medium</t>
+      <c r="L5" s="5" t="inlineStr">
+        <is>
+          <t>Small</t>
         </is>
       </c>
       <c r="M5" s="2" t="n">
         <v>6.5</v>
       </c>
       <c r="N5" s="7" t="n">
-        <v>3.25</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="6">
@@ -788,7 +794,7 @@
         <v>2.217355782608345</v>
       </c>
       <c r="E6" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F6" s="4" t="n">
         <v>0</v>
@@ -797,18 +803,18 @@
         <v>-1.240215946204668</v>
       </c>
       <c r="H6" t="n">
-        <v>1.108677891304173</v>
+        <v>0.9916316520429012</v>
       </c>
       <c r="I6" t="n">
-        <v>-2.480431892409335</v>
+        <v>-2.773207162492859</v>
       </c>
       <c r="J6" t="n">
-        <v>0.04461792188866465</v>
+        <v>0.02508298843768903</v>
       </c>
       <c r="K6" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="L6" s="9" t="inlineStr">
+      <c r="L6" s="8" t="inlineStr">
         <is>
           <t>Very large</t>
         </is>
@@ -816,8 +822,8 @@
       <c r="M6" s="2" t="n">
         <v>4.9</v>
       </c>
-      <c r="N6" s="10" t="n">
-        <v>3.5</v>
+      <c r="N6" s="9" t="n">
+        <v>3.4</v>
       </c>
     </row>
     <row r="7">
@@ -836,22 +842,22 @@
         <v>3.316051302802693</v>
       </c>
       <c r="E7" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F7" s="4" t="n">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="G7" t="n">
-        <v>-0.4457319988352853</v>
+        <v>-0.4608101732765977</v>
       </c>
       <c r="H7" t="n">
-        <v>1.658025651401347</v>
+        <v>1.482983225988712</v>
       </c>
       <c r="I7" t="n">
-        <v>-0.8914639976705706</v>
+        <v>-1.030402872169929</v>
       </c>
       <c r="J7" t="n">
-        <v>0.219178577887749</v>
+        <v>0.1805229210624517</v>
       </c>
       <c r="K7" s="4" t="b">
         <v>0</v>
@@ -865,7 +871,7 @@
         <v>7.9</v>
       </c>
       <c r="N7" s="7" t="n">
-        <v>3.25</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="8">
@@ -884,36 +890,36 @@
         <v>3.374838631159804</v>
       </c>
       <c r="E8" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F8" s="3" t="n">
-        <v>3</v>
+        <v>3.4</v>
       </c>
       <c r="G8" t="n">
-        <v>0.08317486702749352</v>
+        <v>0.2016990525416718</v>
       </c>
       <c r="H8" t="n">
-        <v>1.687419315579902</v>
+        <v>1.509273718473132</v>
       </c>
       <c r="I8" t="n">
-        <v>0.166349734054987</v>
+        <v>0.4510127924804798</v>
       </c>
       <c r="J8" t="n">
-        <v>0.4392306165197497</v>
+        <v>0.337674591265674</v>
       </c>
       <c r="K8" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="L8" s="11" t="inlineStr">
-        <is>
-          <t>Very small</t>
+      <c r="L8" s="5" t="inlineStr">
+        <is>
+          <t>Small</t>
         </is>
       </c>
       <c r="M8" s="2" t="n">
-        <v>7.9</v>
-      </c>
-      <c r="N8" s="12" t="n">
-        <v>3.75</v>
+        <v>7.8</v>
+      </c>
+      <c r="N8" s="10" t="n">
+        <v>3.6</v>
       </c>
     </row>
     <row r="9">
@@ -932,22 +938,22 @@
         <v>2.564204284225516</v>
       </c>
       <c r="E9" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F9" s="3" t="n">
-        <v>3.75</v>
+        <v>3.4</v>
       </c>
       <c r="G9" t="n">
-        <v>0.4190623228107307</v>
+        <v>0.2825677376666641</v>
       </c>
       <c r="H9" t="n">
-        <v>1.282102142112758</v>
+        <v>1.146747017544889</v>
       </c>
       <c r="I9" t="n">
-        <v>0.8381246456214615</v>
+        <v>0.6318406696709888</v>
       </c>
       <c r="J9" t="n">
-        <v>0.2317403732356839</v>
+        <v>0.2809007507751594</v>
       </c>
       <c r="K9" s="4" t="b">
         <v>0</v>
@@ -958,10 +964,10 @@
         </is>
       </c>
       <c r="M9" s="2" t="n">
-        <v>6.1</v>
-      </c>
-      <c r="N9" s="6" t="n">
-        <v>2.75</v>
+        <v>6</v>
+      </c>
+      <c r="N9" s="7" t="n">
+        <v>3.2</v>
       </c>
     </row>
     <row r="10">
@@ -980,36 +986,36 @@
         <v>2.72065363800293</v>
       </c>
       <c r="E10" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F10" s="4" t="n">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="G10" t="n">
-        <v>-0.6529003782993752</v>
+        <v>-0.6345224417250224</v>
       </c>
       <c r="H10" t="n">
-        <v>1.360326819001465</v>
+        <v>1.216713295561331</v>
       </c>
       <c r="I10" t="n">
-        <v>-1.30580075659875</v>
+        <v>-1.418835312946299</v>
       </c>
       <c r="J10" t="n">
-        <v>0.1413641843755108</v>
+        <v>0.1144725903144041</v>
       </c>
       <c r="K10" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="L10" s="8" t="inlineStr">
+      <c r="L10" s="11" t="inlineStr">
         <is>
           <t>Medium</t>
         </is>
       </c>
       <c r="M10" s="2" t="n">
-        <v>5.9</v>
-      </c>
-      <c r="N10" s="6" t="n">
-        <v>2.75</v>
+        <v>5.8</v>
+      </c>
+      <c r="N10" s="7" t="n">
+        <v>3.2</v>
       </c>
     </row>
     <row r="11">
@@ -1028,36 +1034,36 @@
         <v>2.834455750679565</v>
       </c>
       <c r="E11" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F11" s="3" t="n">
-        <v>4.5</v>
+        <v>3.8</v>
       </c>
       <c r="G11" t="n">
-        <v>0.7334555735867889</v>
+        <v>0.4864945829866802</v>
       </c>
       <c r="H11" t="n">
-        <v>1.417227875339782</v>
+        <v>1.267607147546941</v>
       </c>
       <c r="I11" t="n">
-        <v>1.466911147173578</v>
+        <v>1.08783495824363</v>
       </c>
       <c r="J11" t="n">
-        <v>0.1193391218209156</v>
+        <v>0.16891312541507</v>
       </c>
       <c r="K11" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="L11" s="8" t="inlineStr">
-        <is>
-          <t>Medium</t>
+      <c r="L11" s="5" t="inlineStr">
+        <is>
+          <t>Small</t>
         </is>
       </c>
       <c r="M11" s="2" t="n">
-        <v>7.3</v>
+        <v>7.4</v>
       </c>
       <c r="N11" s="7" t="n">
-        <v>3.25</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="12">
@@ -1076,36 +1082,36 @@
         <v>2.796456341019272</v>
       </c>
       <c r="E12" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F12" s="3" t="n">
-        <v>4</v>
+        <v>3.2</v>
       </c>
       <c r="G12" t="n">
-        <v>0.5925867079830219</v>
+        <v>0.3065103661981148</v>
       </c>
       <c r="H12" t="n">
-        <v>1.398228170509636</v>
+        <v>1.250613294925885</v>
       </c>
       <c r="I12" t="n">
-        <v>1.185173415966044</v>
+        <v>0.6853780146273386</v>
       </c>
       <c r="J12" t="n">
-        <v>0.1606389983057708</v>
+        <v>0.2653808961256224</v>
       </c>
       <c r="K12" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="L12" s="8" t="inlineStr">
-        <is>
-          <t>Medium</t>
+      <c r="L12" s="5" t="inlineStr">
+        <is>
+          <t>Small</t>
         </is>
       </c>
       <c r="M12" s="2" t="n">
         <v>7.7</v>
       </c>
-      <c r="N12" s="12" t="n">
-        <v>3.75</v>
+      <c r="N12" s="10" t="n">
+        <v>3.6</v>
       </c>
     </row>
     <row r="13">
@@ -1124,36 +1130,36 @@
         <v>2.887777746459122</v>
       </c>
       <c r="E13" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F13" s="3" t="n">
-        <v>6</v>
+        <v>6.4</v>
       </c>
       <c r="G13" t="n">
-        <v>1.266681530920193</v>
+        <v>1.405196345812185</v>
       </c>
       <c r="H13" t="n">
-        <v>1.443888873229561</v>
+        <v>1.29145346899875</v>
       </c>
       <c r="I13" t="n">
-        <v>2.533363061840385</v>
+        <v>3.142114550970348</v>
       </c>
       <c r="J13" t="n">
-        <v>0.04258640682909735</v>
+        <v>0.01738842788886309</v>
       </c>
       <c r="K13" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="L13" s="9" t="inlineStr">
+      <c r="L13" s="8" t="inlineStr">
         <is>
           <t>Very large</t>
         </is>
       </c>
       <c r="M13" s="2" t="n">
-        <v>6.6</v>
+        <v>6.7</v>
       </c>
       <c r="N13" s="6" t="n">
-        <v>2.75</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="14">
@@ -1172,27 +1178,27 @@
         <v>2.360506647838899</v>
       </c>
       <c r="E14" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F14" s="4" t="n">
-        <v>2</v>
+        <v>1.8</v>
       </c>
       <c r="G14" t="n">
-        <v>-0.1021269856588352</v>
+        <v>-0.1868545589461652</v>
       </c>
       <c r="H14" t="n">
-        <v>1.18025332391945</v>
+        <v>1.055650665181587</v>
       </c>
       <c r="I14" t="n">
-        <v>-0.2042539713176704</v>
+        <v>-0.4178194957093668</v>
       </c>
       <c r="J14" t="n">
-        <v>0.4256133398415425</v>
+        <v>0.3487666635983222</v>
       </c>
       <c r="K14" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="L14" s="11" t="inlineStr">
+      <c r="L14" s="12" t="inlineStr">
         <is>
           <t>Very small</t>
         </is>
@@ -1200,8 +1206,8 @@
       <c r="M14" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="N14" s="7" t="n">
-        <v>3.25</v>
+      <c r="N14" s="13" t="n">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update with GW6 data
</commit_message>
<xml_diff>
--- a/results/Forwards_analysis.xlsx
+++ b/results/Forwards_analysis.xlsx
@@ -67,12 +67,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="0065C2A3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="00228A44"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0065C2A3"/>
       </patternFill>
     </fill>
     <fill>
@@ -82,17 +82,17 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="0040AD75"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="003A855E"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00F2F1F1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00E6979D"/>
+        <fgColor rgb="00EFF2F0"/>
       </patternFill>
     </fill>
     <fill>
@@ -102,7 +102,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0094BCA7"/>
+        <fgColor rgb="00E6959B"/>
       </patternFill>
     </fill>
   </fills>
@@ -133,14 +133,14 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -602,22 +602,22 @@
         <v>4.554709316290477</v>
       </c>
       <c r="E2" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F2" s="3" t="n">
-        <v>7.8</v>
+        <v>7.5</v>
       </c>
       <c r="G2" t="n">
-        <v>0.3720845227254851</v>
+        <v>0.306218628951098</v>
       </c>
       <c r="H2" t="n">
-        <v>2.036927929795419</v>
+        <v>1.859452291935418</v>
       </c>
       <c r="I2" t="n">
-        <v>0.83200628618975</v>
+        <v>0.7500793906648423</v>
       </c>
       <c r="J2" t="n">
-        <v>0.2260961083317141</v>
+        <v>0.2434902368758151</v>
       </c>
       <c r="K2" s="4" t="b">
         <v>0</v>
@@ -631,7 +631,7 @@
         <v>14.1</v>
       </c>
       <c r="N2" s="6" t="n">
-        <v>2.8</v>
+        <v>2.833333333333333</v>
       </c>
     </row>
     <row r="3">
@@ -650,22 +650,22 @@
         <v>2.851061463238469</v>
       </c>
       <c r="E3" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F3" s="3" t="n">
-        <v>4.4</v>
+        <v>4.666666666666667</v>
       </c>
       <c r="G3" t="n">
-        <v>0.2695210406859287</v>
+        <v>0.3630534566317305</v>
       </c>
       <c r="H3" t="n">
-        <v>1.275033447966247</v>
+        <v>1.163940968374505</v>
       </c>
       <c r="I3" t="n">
-        <v>0.6026673683402233</v>
+        <v>0.8892957181014012</v>
       </c>
       <c r="J3" t="n">
-        <v>0.2896149239936908</v>
+        <v>0.2072883292816573</v>
       </c>
       <c r="K3" s="4" t="b">
         <v>0</v>
@@ -676,10 +676,10 @@
         </is>
       </c>
       <c r="M3" s="2" t="n">
-        <v>8</v>
+        <v>7.9</v>
       </c>
       <c r="N3" s="7" t="n">
-        <v>3.2</v>
+        <v>3.166666666666667</v>
       </c>
     </row>
     <row r="4">
@@ -698,22 +698,22 @@
         <v>2.83492443229031</v>
       </c>
       <c r="E4" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F4" s="4" t="n">
-        <v>2.2</v>
+        <v>2</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.3944309080854226</v>
+        <v>-0.4649795257917584</v>
       </c>
       <c r="H4" t="n">
-        <v>1.267816748335227</v>
+        <v>1.157353053076757</v>
       </c>
       <c r="I4" t="n">
-        <v>-0.8819743229059763</v>
+        <v>-1.138962579031098</v>
       </c>
       <c r="J4" t="n">
-        <v>0.2138016944959831</v>
+        <v>0.153164179321003</v>
       </c>
       <c r="K4" s="4" t="b">
         <v>0</v>
@@ -727,7 +727,7 @@
         <v>7.3</v>
       </c>
       <c r="N4" s="7" t="n">
-        <v>3.2</v>
+        <v>3.166666666666667</v>
       </c>
     </row>
     <row r="5">
@@ -746,36 +746,36 @@
         <v>2.846974386589162</v>
       </c>
       <c r="E5" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F5" s="3" t="n">
-        <v>4.2</v>
+        <v>4.5</v>
       </c>
       <c r="G5" t="n">
-        <v>0.4030132573223619</v>
+        <v>0.5083882833194932</v>
       </c>
       <c r="H5" t="n">
-        <v>1.273205651722827</v>
+        <v>1.162272426319431</v>
       </c>
       <c r="I5" t="n">
-        <v>0.9011650392064161</v>
+        <v>1.245291885342247</v>
       </c>
       <c r="J5" t="n">
-        <v>0.2092273859615639</v>
+        <v>0.134100706077421</v>
       </c>
       <c r="K5" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="L5" s="5" t="inlineStr">
-        <is>
-          <t>Small</t>
+      <c r="L5" s="8" t="inlineStr">
+        <is>
+          <t>Medium</t>
         </is>
       </c>
       <c r="M5" s="2" t="n">
-        <v>6.5</v>
+        <v>6.4</v>
       </c>
       <c r="N5" s="7" t="n">
-        <v>3.2</v>
+        <v>3.166666666666667</v>
       </c>
     </row>
     <row r="6">
@@ -794,7 +794,7 @@
         <v>2.217355782608345</v>
       </c>
       <c r="E6" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F6" s="4" t="n">
         <v>0</v>
@@ -803,18 +803,18 @@
         <v>-1.240215946204668</v>
       </c>
       <c r="H6" t="n">
-        <v>0.9916316520429012</v>
+        <v>0.9052317076000181</v>
       </c>
       <c r="I6" t="n">
-        <v>-2.773207162492859</v>
+        <v>-3.037896239064466</v>
       </c>
       <c r="J6" t="n">
-        <v>0.02508298843768903</v>
+        <v>0.01440999036614293</v>
       </c>
       <c r="K6" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="L6" s="8" t="inlineStr">
+      <c r="L6" s="9" t="inlineStr">
         <is>
           <t>Very large</t>
         </is>
@@ -822,8 +822,8 @@
       <c r="M6" s="2" t="n">
         <v>4.9</v>
       </c>
-      <c r="N6" s="9" t="n">
-        <v>3.4</v>
+      <c r="N6" s="10" t="n">
+        <v>3.5</v>
       </c>
     </row>
     <row r="7">
@@ -842,22 +842,22 @@
         <v>3.316051302802693</v>
       </c>
       <c r="E7" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F7" s="4" t="n">
-        <v>1.2</v>
+        <v>1.333333333333333</v>
       </c>
       <c r="G7" t="n">
-        <v>-0.4608101732765977</v>
+        <v>-0.4206017080997648</v>
       </c>
       <c r="H7" t="n">
-        <v>1.482983225988712</v>
+        <v>1.353772275459665</v>
       </c>
       <c r="I7" t="n">
-        <v>-1.030402872169929</v>
+        <v>-1.030259569787458</v>
       </c>
       <c r="J7" t="n">
-        <v>0.1805229210624517</v>
+        <v>0.1750615400789786</v>
       </c>
       <c r="K7" s="4" t="b">
         <v>0</v>
@@ -871,7 +871,7 @@
         <v>7.9</v>
       </c>
       <c r="N7" s="7" t="n">
-        <v>3.2</v>
+        <v>3.166666666666667</v>
       </c>
     </row>
     <row r="8">
@@ -890,22 +890,22 @@
         <v>3.374838631159804</v>
       </c>
       <c r="E8" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F8" s="3" t="n">
-        <v>3.4</v>
+        <v>3.833333333333333</v>
       </c>
       <c r="G8" t="n">
-        <v>0.2016990525416718</v>
+        <v>0.3301002535153649</v>
       </c>
       <c r="H8" t="n">
-        <v>1.509273718473132</v>
+        <v>1.377772101762393</v>
       </c>
       <c r="I8" t="n">
-        <v>0.4510127924804798</v>
+        <v>0.8085771850760132</v>
       </c>
       <c r="J8" t="n">
-        <v>0.337674591265674</v>
+        <v>0.2277467504197668</v>
       </c>
       <c r="K8" s="4" t="b">
         <v>0</v>
@@ -918,8 +918,8 @@
       <c r="M8" s="2" t="n">
         <v>7.8</v>
       </c>
-      <c r="N8" s="10" t="n">
-        <v>3.6</v>
+      <c r="N8" s="11" t="n">
+        <v>3.333333333333333</v>
       </c>
     </row>
     <row r="9">
@@ -938,36 +938,36 @@
         <v>2.564204284225516</v>
       </c>
       <c r="E9" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F9" s="3" t="n">
-        <v>3.4</v>
+        <v>3.166666666666667</v>
       </c>
       <c r="G9" t="n">
-        <v>0.2825677376666641</v>
+        <v>0.1915713475706197</v>
       </c>
       <c r="H9" t="n">
-        <v>1.146747017544889</v>
+        <v>1.04683201543518</v>
       </c>
       <c r="I9" t="n">
-        <v>0.6318406696709888</v>
+        <v>0.469252050885384</v>
       </c>
       <c r="J9" t="n">
-        <v>0.2809007507751594</v>
+        <v>0.3293196862112076</v>
       </c>
       <c r="K9" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="L9" s="5" t="inlineStr">
-        <is>
-          <t>Small</t>
+      <c r="L9" s="12" t="inlineStr">
+        <is>
+          <t>Very small</t>
         </is>
       </c>
       <c r="M9" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="N9" s="7" t="n">
-        <v>3.2</v>
+      <c r="N9" s="11" t="n">
+        <v>3.333333333333333</v>
       </c>
     </row>
     <row r="10">
@@ -986,27 +986,27 @@
         <v>2.72065363800293</v>
       </c>
       <c r="E10" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F10" s="4" t="n">
-        <v>0.8</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="G10" t="n">
-        <v>-0.6345224417250224</v>
+        <v>-0.6222704840087872</v>
       </c>
       <c r="H10" t="n">
-        <v>1.216713295561331</v>
+        <v>1.110702196658986</v>
       </c>
       <c r="I10" t="n">
-        <v>-1.418835312946299</v>
+        <v>-1.524245167816248</v>
       </c>
       <c r="J10" t="n">
-        <v>0.1144725903144041</v>
+        <v>0.09397796480394355</v>
       </c>
       <c r="K10" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="L10" s="11" t="inlineStr">
+      <c r="L10" s="8" t="inlineStr">
         <is>
           <t>Medium</t>
         </is>
@@ -1014,8 +1014,8 @@
       <c r="M10" s="2" t="n">
         <v>5.8</v>
       </c>
-      <c r="N10" s="7" t="n">
-        <v>3.2</v>
+      <c r="N10" s="11" t="n">
+        <v>3.333333333333333</v>
       </c>
     </row>
     <row r="11">
@@ -1034,36 +1034,36 @@
         <v>2.834455750679565</v>
       </c>
       <c r="E11" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F11" s="3" t="n">
-        <v>3.8</v>
+        <v>4.166666666666667</v>
       </c>
       <c r="G11" t="n">
-        <v>0.4864945829866802</v>
+        <v>0.6158551018724515</v>
       </c>
       <c r="H11" t="n">
-        <v>1.267607147546941</v>
+        <v>1.157161714610398</v>
       </c>
       <c r="I11" t="n">
-        <v>1.08783495824363</v>
+        <v>1.508530755077259</v>
       </c>
       <c r="J11" t="n">
-        <v>0.16891312541507</v>
+        <v>0.095895221785726</v>
       </c>
       <c r="K11" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="L11" s="5" t="inlineStr">
-        <is>
-          <t>Small</t>
+      <c r="L11" s="8" t="inlineStr">
+        <is>
+          <t>Medium</t>
         </is>
       </c>
       <c r="M11" s="2" t="n">
         <v>7.4</v>
       </c>
       <c r="N11" s="7" t="n">
-        <v>3.2</v>
+        <v>3.166666666666667</v>
       </c>
     </row>
     <row r="12">
@@ -1082,22 +1082,22 @@
         <v>2.796456341019272</v>
       </c>
       <c r="E12" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F12" s="3" t="n">
-        <v>3.2</v>
+        <v>3.5</v>
       </c>
       <c r="G12" t="n">
-        <v>0.3065103661981148</v>
+        <v>0.413788994367455</v>
       </c>
       <c r="H12" t="n">
-        <v>1.250613294925885</v>
+        <v>1.141648520577947</v>
       </c>
       <c r="I12" t="n">
-        <v>0.6853780146273386</v>
+        <v>1.013571897379647</v>
       </c>
       <c r="J12" t="n">
-        <v>0.2653808961256224</v>
+        <v>0.1786474632144996</v>
       </c>
       <c r="K12" s="4" t="b">
         <v>0</v>
@@ -1108,10 +1108,10 @@
         </is>
       </c>
       <c r="M12" s="2" t="n">
-        <v>7.7</v>
-      </c>
-      <c r="N12" s="10" t="n">
-        <v>3.6</v>
+        <v>7.6</v>
+      </c>
+      <c r="N12" s="11" t="n">
+        <v>3.333333333333333</v>
       </c>
     </row>
     <row r="13">
@@ -1130,36 +1130,36 @@
         <v>2.887777746459122</v>
       </c>
       <c r="E13" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F13" s="3" t="n">
-        <v>6.4</v>
+        <v>5.5</v>
       </c>
       <c r="G13" t="n">
-        <v>1.405196345812185</v>
+        <v>1.093538012305202</v>
       </c>
       <c r="H13" t="n">
-        <v>1.29145346899875</v>
+        <v>1.178930328231524</v>
       </c>
       <c r="I13" t="n">
-        <v>3.142114550970348</v>
+        <v>2.678610144485098</v>
       </c>
       <c r="J13" t="n">
-        <v>0.01738842788886309</v>
+        <v>0.0219465755021444</v>
       </c>
       <c r="K13" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="L13" s="8" t="inlineStr">
-        <is>
-          <t>Very large</t>
+      <c r="L13" s="13" t="inlineStr">
+        <is>
+          <t>Large</t>
         </is>
       </c>
       <c r="M13" s="2" t="n">
-        <v>6.7</v>
+        <v>6.9</v>
       </c>
       <c r="N13" s="6" t="n">
-        <v>2.8</v>
+        <v>2.833333333333333</v>
       </c>
     </row>
     <row r="14">
@@ -1178,36 +1178,36 @@
         <v>2.360506647838899</v>
       </c>
       <c r="E14" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F14" s="4" t="n">
-        <v>1.8</v>
+        <v>1.666666666666667</v>
       </c>
       <c r="G14" t="n">
-        <v>-0.1868545589461652</v>
+        <v>-0.2433396078043851</v>
       </c>
       <c r="H14" t="n">
-        <v>1.055650665181587</v>
+        <v>0.9636728036088147</v>
       </c>
       <c r="I14" t="n">
-        <v>-0.4178194957093668</v>
+        <v>-0.5960578733297227</v>
       </c>
       <c r="J14" t="n">
-        <v>0.3487666635983222</v>
+        <v>0.2885464810659479</v>
       </c>
       <c r="K14" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="L14" s="12" t="inlineStr">
-        <is>
-          <t>Very small</t>
+      <c r="L14" s="5" t="inlineStr">
+        <is>
+          <t>Small</t>
         </is>
       </c>
       <c r="M14" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="N14" s="13" t="n">
-        <v>3</v>
+      <c r="N14" s="11" t="n">
+        <v>3.333333333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>